<commit_message>
full repvgg block implemented
</commit_message>
<xml_diff>
--- a/experiment/fig1/data.xlsx
+++ b/experiment/fig1/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0690DA-5CB9-4D59-A56D-51BCEB2AFFE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264DD6FB-47DF-4623-B5F8-010814701125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,10 @@
     <sheet name="ablation_init" sheetId="8" r:id="rId5"/>
     <sheet name="ablation_repvgg" sheetId="9" r:id="rId6"/>
     <sheet name="ablation_distill" sheetId="10" r:id="rId7"/>
-    <sheet name="x2" sheetId="4" r:id="rId8"/>
-    <sheet name="x3" sheetId="5" r:id="rId9"/>
-    <sheet name="x4" sheetId="6" r:id="rId10"/>
+    <sheet name="Ablation" sheetId="11" r:id="rId8"/>
+    <sheet name="x2" sheetId="4" r:id="rId9"/>
+    <sheet name="x3" sheetId="5" r:id="rId10"/>
+    <sheet name="x4" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="593">
   <si>
     <t>Model name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1832,13 +1833,48 @@
   </si>
   <si>
     <t>seed=236</t>
+  </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plain-m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>init_stu</t>
+  </si>
+  <si>
+    <t>dist_coe</t>
+  </si>
+  <si>
+    <t>init_dist</t>
+  </si>
+  <si>
+    <t>decompose_adjust</t>
+  </si>
+  <si>
+    <t>Set5</t>
+  </si>
+  <si>
+    <t>Set14</t>
+  </si>
+  <si>
+    <t>B100</t>
+  </si>
+  <si>
+    <t>Urban100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1866,6 +1902,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF212121"/>
       <name val="Arial"/>
@@ -1925,7 +1968,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1949,6 +1992,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2399,6 +2445,540 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E4D1BB-A6AD-4902-AB06-A0EF0E8DC8B7}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col min="9" max="9" width="18.75" customWidth="1"/>
+    <col min="10" max="10" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10" t="s">
+        <v>155</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J22">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E89D0B4-1B01-4C9B-B949-158A53C19AFB}">
   <dimension ref="A1:J21"/>
   <sheetViews>
@@ -5201,10 +5781,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6210ED35-9BF5-4DB7-A1FB-312D2FE75AD2}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5408,10 +5988,97 @@
         <v>576</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="C10" s="7">
+        <v>37.588000000000001</v>
+      </c>
+      <c r="D10" s="7">
+        <v>33.199199999999998</v>
+      </c>
+      <c r="E10" s="7">
+        <v>31.921299999999999</v>
+      </c>
+      <c r="F10" s="7">
+        <v>31.092500000000001</v>
+      </c>
+      <c r="G10" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C11" s="7">
+        <v>37.585999999999999</v>
+      </c>
+      <c r="D11" s="7">
+        <v>33.200499999999998</v>
+      </c>
+      <c r="E11" s="7">
+        <v>31.918299999999999</v>
+      </c>
+      <c r="F11" s="7">
+        <v>31.096800000000002</v>
+      </c>
+      <c r="G11" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="C12" s="7">
+        <v>37.593499999999999</v>
+      </c>
+      <c r="D12" s="7">
+        <v>33.191499999999998</v>
+      </c>
+      <c r="E12" s="7">
+        <v>31.9175</v>
+      </c>
+      <c r="F12" s="7">
+        <v>31.070499999999999</v>
+      </c>
+      <c r="G12" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="C13" s="7">
+        <v>37.587000000000003</v>
+      </c>
+      <c r="D13" s="7">
+        <v>33.1843</v>
+      </c>
+      <c r="E13" s="7">
+        <v>31.9068</v>
+      </c>
+      <c r="F13" s="7">
+        <v>31.049499999999998</v>
+      </c>
+      <c r="G13" t="s">
+        <v>576</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5460,15 +6127,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987EE552-3FB2-4803-9EF9-132E2CA87291}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>209</v>
       </c>
@@ -5490,8 +6157,11 @@
       <c r="G1" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>4</v>
       </c>
@@ -5513,8 +6183,11 @@
       <c r="G2" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>577</v>
@@ -5534,8 +6207,11 @@
       <c r="G3" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>577</v>
@@ -5555,8 +6231,11 @@
       <c r="G4" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>577</v>
@@ -5576,26 +6255,29 @@
       <c r="G5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5607,10 +6289,1117 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77F8BA6-364B-4310-A067-116A9788ACD9}">
+  <dimension ref="A1:J46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>31.579000000000001</v>
+      </c>
+      <c r="G2" s="7">
+        <v>28.222999999999999</v>
+      </c>
+      <c r="H2" s="7">
+        <v>27.312000000000001</v>
+      </c>
+      <c r="I2" s="7">
+        <v>25.306000000000001</v>
+      </c>
+      <c r="J2" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>64</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7">
+        <v>31.579000000000001</v>
+      </c>
+      <c r="G3" s="7">
+        <v>28.222999999999999</v>
+      </c>
+      <c r="H3" s="7">
+        <v>27.312000000000001</v>
+      </c>
+      <c r="I3" s="7">
+        <v>25.306000000000001</v>
+      </c>
+      <c r="J3" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>31.579000000000001</v>
+      </c>
+      <c r="G4" s="7">
+        <v>28.222999999999999</v>
+      </c>
+      <c r="H4" s="7">
+        <v>27.312000000000001</v>
+      </c>
+      <c r="I4" s="7">
+        <v>25.306000000000001</v>
+      </c>
+      <c r="J4" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>31.579000000000001</v>
+      </c>
+      <c r="G5" s="7">
+        <v>28.222999999999999</v>
+      </c>
+      <c r="H5" s="7">
+        <v>27.312000000000001</v>
+      </c>
+      <c r="I5" s="7">
+        <v>25.306000000000001</v>
+      </c>
+      <c r="J5" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>31.853000000000002</v>
+      </c>
+      <c r="G6" s="7">
+        <v>28.4</v>
+      </c>
+      <c r="H6" s="7">
+        <v>27.434000000000001</v>
+      </c>
+      <c r="I6" s="7">
+        <v>25.658000000000001</v>
+      </c>
+      <c r="J6" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>64</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="G7" s="7">
+        <v>28.379000000000001</v>
+      </c>
+      <c r="H7" s="7">
+        <v>27.422000000000001</v>
+      </c>
+      <c r="I7" s="7">
+        <v>25.614999999999998</v>
+      </c>
+      <c r="J7" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>64</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>31.853000000000002</v>
+      </c>
+      <c r="G8" s="7">
+        <v>28.4</v>
+      </c>
+      <c r="H8" s="7">
+        <v>27.434000000000001</v>
+      </c>
+      <c r="I8" s="7">
+        <v>25.658000000000001</v>
+      </c>
+      <c r="J8" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>28.379000000000001</v>
+      </c>
+      <c r="H9" s="7">
+        <v>27.422000000000001</v>
+      </c>
+      <c r="I9" s="7">
+        <v>25.614999999999998</v>
+      </c>
+      <c r="J9" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>64</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>31.984000000000002</v>
+      </c>
+      <c r="G10" s="7">
+        <v>28.513999999999999</v>
+      </c>
+      <c r="H10" s="7">
+        <v>27.516999999999999</v>
+      </c>
+      <c r="I10" s="7">
+        <v>25.917000000000002</v>
+      </c>
+      <c r="J10" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3</v>
+      </c>
+      <c r="F11" s="7">
+        <v>32.116999999999997</v>
+      </c>
+      <c r="G11" s="7">
+        <v>28.538</v>
+      </c>
+      <c r="H11" s="7">
+        <v>27.533000000000001</v>
+      </c>
+      <c r="I11" s="7">
+        <v>25.965</v>
+      </c>
+      <c r="J11" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>64</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>31.984000000000002</v>
+      </c>
+      <c r="G12" s="7">
+        <v>28.513999999999999</v>
+      </c>
+      <c r="H12" s="7">
+        <v>27.516999999999999</v>
+      </c>
+      <c r="I12" s="7">
+        <v>25.917000000000002</v>
+      </c>
+      <c r="J12" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>64</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
+        <v>32.116999999999997</v>
+      </c>
+      <c r="G13" s="7">
+        <v>28.538</v>
+      </c>
+      <c r="H13" s="7">
+        <v>27.533000000000001</v>
+      </c>
+      <c r="I13" s="7">
+        <v>25.965</v>
+      </c>
+      <c r="J13" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>64</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>32.048999999999999</v>
+      </c>
+      <c r="G14" s="7">
+        <v>28.489000000000001</v>
+      </c>
+      <c r="H14" s="7">
+        <v>27.552</v>
+      </c>
+      <c r="I14" s="7">
+        <v>25.98</v>
+      </c>
+      <c r="J14" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>64</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7">
+        <v>32.085000000000001</v>
+      </c>
+      <c r="G15" s="7">
+        <v>28.553000000000001</v>
+      </c>
+      <c r="H15" s="7">
+        <v>27.552</v>
+      </c>
+      <c r="I15" s="7">
+        <v>25.992000000000001</v>
+      </c>
+      <c r="J15" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>64</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>32.093000000000004</v>
+      </c>
+      <c r="G16" s="7">
+        <v>28.559000000000001</v>
+      </c>
+      <c r="H16" s="7">
+        <v>27.552</v>
+      </c>
+      <c r="I16" s="7">
+        <v>25.962</v>
+      </c>
+      <c r="J16" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>64</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>3</v>
+      </c>
+      <c r="F17" s="7">
+        <v>32.085000000000001</v>
+      </c>
+      <c r="G17" s="7">
+        <v>28.553000000000001</v>
+      </c>
+      <c r="H17" s="7">
+        <v>27.552</v>
+      </c>
+      <c r="I17" s="7">
+        <v>25.992000000000001</v>
+      </c>
+      <c r="J17" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>64</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>31.619</v>
+      </c>
+      <c r="G18" s="7">
+        <v>28.248000000000001</v>
+      </c>
+      <c r="H18" s="7">
+        <v>27.327999999999999</v>
+      </c>
+      <c r="I18" s="7">
+        <v>25.35</v>
+      </c>
+      <c r="J18" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>64</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>32.063000000000002</v>
+      </c>
+      <c r="G19" s="7">
+        <v>28.52</v>
+      </c>
+      <c r="H19" s="7">
+        <v>27.518999999999998</v>
+      </c>
+      <c r="I19" s="7">
+        <v>25.9</v>
+      </c>
+      <c r="J19" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>64</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>31.625</v>
+      </c>
+      <c r="G20" s="7">
+        <v>28.25</v>
+      </c>
+      <c r="H20" s="7">
+        <v>27.323</v>
+      </c>
+      <c r="I20" s="7">
+        <v>25.343</v>
+      </c>
+      <c r="J20" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>64</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
+        <v>32.023000000000003</v>
+      </c>
+      <c r="G21" s="7">
+        <v>28.513999999999999</v>
+      </c>
+      <c r="H21" s="7">
+        <v>27.523</v>
+      </c>
+      <c r="I21" s="7">
+        <v>25.907</v>
+      </c>
+      <c r="J21" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>64</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
+        <v>31.844999999999999</v>
+      </c>
+      <c r="G22" s="7">
+        <v>28.376999999999999</v>
+      </c>
+      <c r="H22" s="7">
+        <v>27.437000000000001</v>
+      </c>
+      <c r="I22" s="7">
+        <v>25.675999999999998</v>
+      </c>
+      <c r="J22" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>64</v>
+      </c>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7">
+        <v>32.119</v>
+      </c>
+      <c r="G23" s="7">
+        <v>28.542000000000002</v>
+      </c>
+      <c r="H23" s="7">
+        <v>27.544</v>
+      </c>
+      <c r="I23" s="7">
+        <v>25.974</v>
+      </c>
+      <c r="J23" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>64</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
+        <v>31.824000000000002</v>
+      </c>
+      <c r="G24" s="7">
+        <v>28.401</v>
+      </c>
+      <c r="H24" s="7">
+        <v>27.443000000000001</v>
+      </c>
+      <c r="I24" s="7">
+        <v>25.675000000000001</v>
+      </c>
+      <c r="J24" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>64</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>32.112000000000002</v>
+      </c>
+      <c r="G25" s="7">
+        <v>28.56</v>
+      </c>
+      <c r="H25" s="7">
+        <v>27.545999999999999</v>
+      </c>
+      <c r="I25" s="7">
+        <v>25.952999999999999</v>
+      </c>
+      <c r="J25" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>64</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>3</v>
+      </c>
+      <c r="F26" s="7">
+        <v>31.619</v>
+      </c>
+      <c r="G26" s="7">
+        <v>28.248000000000001</v>
+      </c>
+      <c r="H26" s="7">
+        <v>27.327999999999999</v>
+      </c>
+      <c r="I26" s="7">
+        <v>25.35</v>
+      </c>
+      <c r="J26" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>64</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>3</v>
+      </c>
+      <c r="F27" s="7">
+        <v>32.103999999999999</v>
+      </c>
+      <c r="G27" s="7">
+        <v>28.524000000000001</v>
+      </c>
+      <c r="H27" s="7">
+        <v>27.53</v>
+      </c>
+      <c r="I27" s="7">
+        <v>25.954999999999998</v>
+      </c>
+      <c r="J27" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>64</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7">
+        <v>3</v>
+      </c>
+      <c r="F28" s="7">
+        <v>31.619</v>
+      </c>
+      <c r="G28" s="7">
+        <v>28.248000000000001</v>
+      </c>
+      <c r="H28" s="7">
+        <v>27.327999999999999</v>
+      </c>
+      <c r="I28" s="7">
+        <v>25.35</v>
+      </c>
+      <c r="J28" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>64</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7">
+        <v>3</v>
+      </c>
+      <c r="F29" s="7">
+        <v>32.043999999999997</v>
+      </c>
+      <c r="G29" s="7">
+        <v>28.547000000000001</v>
+      </c>
+      <c r="H29" s="7">
+        <v>27.527999999999999</v>
+      </c>
+      <c r="I29" s="7">
+        <v>25.968</v>
+      </c>
+      <c r="J29" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>64</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0</v>
+      </c>
+      <c r="C30" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>3</v>
+      </c>
+      <c r="F30" s="7">
+        <v>31.84</v>
+      </c>
+      <c r="G30" s="7">
+        <v>28.366</v>
+      </c>
+      <c r="H30" s="7">
+        <v>27.419</v>
+      </c>
+      <c r="I30" s="7">
+        <v>25.603999999999999</v>
+      </c>
+      <c r="J30" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>64</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>3</v>
+      </c>
+      <c r="F31" s="7">
+        <v>32.113999999999997</v>
+      </c>
+      <c r="G31" s="7">
+        <v>28.556000000000001</v>
+      </c>
+      <c r="H31" s="7">
+        <v>27.547999999999998</v>
+      </c>
+      <c r="I31" s="7">
+        <v>25.992000000000001</v>
+      </c>
+      <c r="J31" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>64</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0</v>
+      </c>
+      <c r="C32" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
+        <v>3</v>
+      </c>
+      <c r="F32" s="7">
+        <v>31.84</v>
+      </c>
+      <c r="G32" s="7">
+        <v>28.366</v>
+      </c>
+      <c r="H32" s="7">
+        <v>27.419</v>
+      </c>
+      <c r="I32" s="7">
+        <v>25.603999999999999</v>
+      </c>
+      <c r="J32" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>64</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7">
+        <v>3</v>
+      </c>
+      <c r="F33" s="7">
+        <v>32.11</v>
+      </c>
+      <c r="G33" s="7">
+        <v>28.565999999999999</v>
+      </c>
+      <c r="H33" s="7">
+        <v>27.547999999999998</v>
+      </c>
+      <c r="I33" s="7">
+        <v>25.983000000000001</v>
+      </c>
+      <c r="J33" s="7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EE7E9B-E9C4-4E46-9F76-B4CCDCFCCCE5}">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -6244,538 +8033,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E4D1BB-A6AD-4902-AB06-A0EF0E8DC8B7}">
-  <dimension ref="A1:J19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="11.75" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
-    <col min="9" max="9" width="18.75" customWidth="1"/>
-    <col min="10" max="10" width="20.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="D8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" t="s">
-        <v>138</v>
-      </c>
-      <c r="G9" t="s">
-        <v>139</v>
-      </c>
-      <c r="H9" t="s">
-        <v>140</v>
-      </c>
-      <c r="I9" t="s">
-        <v>141</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G10" t="s">
-        <v>153</v>
-      </c>
-      <c r="H10" t="s">
-        <v>154</v>
-      </c>
-      <c r="I10" t="s">
-        <v>155</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>493</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" t="s">
-        <v>146</v>
-      </c>
-      <c r="H17" t="s">
-        <v>147</v>
-      </c>
-      <c r="I17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:J22">
-    <sortCondition ref="A2"/>
-  </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>